<commit_message>
Updated FilterInformationFromERTMSTrackside document and diagrams exports.
</commit_message>
<xml_diff>
--- a/System Analysis/WorkingRepository/Group1/FilterInformationFromERTMSTrackside.xlsx
+++ b/System Analysis/WorkingRepository/Group1/FilterInformationFromERTMSTrackside.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="14115" windowHeight="6720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="14115" windowHeight="6720"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="176">
   <si>
     <t>Template for System Analysis</t>
   </si>
@@ -670,6 +670,12 @@
   <si>
     <t xml:space="preserve">3.16.3.3.3.1
 </t>
+  </si>
+  <si>
+    <t>At implementation level, the interactions of the « filter information from ERTMS trackside » function with the other macro functions of ETCS kernel are represented in the Internal Block Diagram shown below.</t>
+  </si>
+  <si>
+    <t>20/11/2013 - v4 - added SysML diagrams</t>
   </si>
 </sst>
 </file>
@@ -936,7 +942,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1045,6 +1051,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1057,6 +1072,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>7</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>173151</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>3338109</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 3" descr="FilterInformationFromERTMSTrackside_Interfaces.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7" y="7343787"/>
+          <a:ext cx="5507144" cy="3328572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1344,10 +1402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1418,88 +1476,119 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" ht="18.75">
-      <c r="A17" s="2" t="s">
+      <c r="A16" s="19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15.75">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" ht="18.75">
+      <c r="A18" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" ht="16.5">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:13" ht="15.75">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" ht="16.5">
+      <c r="A20" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="16.5">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" ht="16.5">
+    <row r="21" spans="1:13" ht="16.5">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="18.75">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:13" ht="16.5">
+      <c r="A22" s="3"/>
+    </row>
+    <row r="23" spans="1:13" ht="18.75">
+      <c r="A23" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="18.75">
-      <c r="A23" s="2"/>
-    </row>
-    <row r="24" spans="1:5" ht="16.5">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:13" ht="18.75">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:13" ht="16.5">
+      <c r="A25" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75">
-      <c r="A25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" ht="18.75">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:13" ht="15.75">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:13" ht="18.75">
+      <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="18.75">
-      <c r="A27" s="4"/>
-    </row>
-    <row r="28" spans="1:5" ht="118.5" customHeight="1">
-      <c r="A28" s="29" t="s">
+    <row r="28" spans="1:13" ht="18.75">
+      <c r="A28" s="4"/>
+    </row>
+    <row r="29" spans="1:13" ht="118.5" customHeight="1">
+      <c r="A29" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-    </row>
-    <row r="29" spans="1:5" ht="15.75">
-      <c r="A29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" ht="15.75">
-      <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" ht="18.75">
-      <c r="A31" s="2" t="s">
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="40"/>
+    </row>
+    <row r="30" spans="1:13" ht="69.75" customHeight="1">
+      <c r="A30" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="38"/>
+    </row>
+    <row r="31" spans="1:13" ht="263.25" customHeight="1">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:13" ht="15.75">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1" ht="18.75">
+      <c r="A33" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A30:E30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1510,7 +1599,7 @@
   </sheetPr>
   <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1260" topLeftCell="A63" activePane="bottomLeft"/>
       <selection activeCell="I1" sqref="I1:I1048576"/>
       <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
@@ -3310,17 +3399,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="G1:G2"/>
@@ -3328,6 +3406,17 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated FilterInfo document with IBD.
Linked fixed data to requirements in the StoreConfig document.
</commit_message>
<xml_diff>
--- a/System Analysis/WorkingRepository/Group1/FilterInformationFromERTMSTrackside.xlsx
+++ b/System Analysis/WorkingRepository/Group1/FilterInformationFromERTMSTrackside.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="14115" windowHeight="6720"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="14115" windowHeight="6720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -1021,6 +1021,15 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1049,15 +1058,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1106,6 +1106,87 @@
         <a:xfrm>
           <a:off x="7" y="7343787"/>
           <a:ext cx="5507144" cy="3328572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1999208</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>8976</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1" descr="FilterInformationFromERTMSTrackside_IBD.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="47405925"/>
+          <a:ext cx="8342858" cy="4390476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>56547</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>694070</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>95358</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2" descr="BuildBGMsgAndUseBGAsRefLoc.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="52224972"/>
+          <a:ext cx="10047620" cy="3848811"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1404,22 +1485,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:7" ht="15.75">
       <c r="A2" s="1"/>
@@ -1527,37 +1608,37 @@
       <c r="A28" s="4"/>
     </row>
     <row r="29" spans="1:13" ht="118.5" customHeight="1">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
-      <c r="K29" s="40"/>
-      <c r="L29" s="40"/>
-      <c r="M29" s="40"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="30"/>
     </row>
     <row r="30" spans="1:13" ht="69.75" customHeight="1">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="38"/>
-      <c r="M30" s="38"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="28"/>
     </row>
     <row r="31" spans="1:13" ht="263.25" customHeight="1">
       <c r="A31" s="1"/>
@@ -1599,10 +1680,10 @@
   </sheetPr>
   <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1260" topLeftCell="A63" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1260" topLeftCell="A94" activePane="bottomLeft"/>
       <selection activeCell="I1" sqref="I1:I1048576"/>
-      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
+      <selection pane="bottomLeft" activeCell="H105" sqref="H105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1652,16 +1733,16 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="33" t="s">
         <v>23</v>
       </c>
       <c r="E2" s="11" t="s">
@@ -1677,18 +1758,18 @@
         <v>22</v>
       </c>
       <c r="I2" s="11"/>
-      <c r="J2" s="30" t="s">
+      <c r="J2" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="33" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="31"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="11" t="s">
         <v>26</v>
       </c>
@@ -1702,8 +1783,8 @@
         <v>26</v>
       </c>
       <c r="I3" s="11"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
     </row>
     <row r="4" spans="1:11" ht="71.25" customHeight="1">
       <c r="A4" s="14"/>
@@ -2843,6 +2924,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="52" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2893,28 +2975,28 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="33" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="33" t="s">
         <v>25</v>
       </c>
       <c r="I2" s="12" t="s">
@@ -2922,31 +3004,31 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
       <c r="I3" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9">
@@ -3128,73 +3210,73 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="37" t="s">
         <v>37</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="L1" s="37" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="16.5" thickBot="1">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
       <c r="H2" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="35"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
     </row>
     <row r="3" spans="1:12" ht="31.5">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="33" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="33" t="s">
         <v>23</v>
       </c>
       <c r="F3" s="10" t="s">
@@ -3209,24 +3291,24 @@
       <c r="I3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="32" t="s">
+      <c r="J3" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="30" t="s">
+      <c r="K3" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="30" t="s">
+      <c r="L3" s="33" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
       <c r="F4" s="10" t="s">
         <v>26</v>
       </c>
@@ -3239,9 +3321,9 @@
       <c r="I4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="33"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="14"/>
@@ -3399,6 +3481,17 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="G1:G2"/>
@@ -3406,17 +3499,6 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3464,25 +3546,25 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="33" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="33" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="12" t="s">
@@ -3490,29 +3572,29 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="31.5" customHeight="1">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
       <c r="H3" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
       <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:8">
@@ -3683,28 +3765,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="33" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
     </row>
     <row r="5" spans="1:5" ht="15.75">
       <c r="A5" s="17" t="s">

</xml_diff>

<commit_message>
Updated diagram images and document for Filter Information from ERTMS Trackside.
</commit_message>
<xml_diff>
--- a/System Analysis/WorkingRepository/Group1/FilterInformationFromERTMSTrackside.xlsx
+++ b/System Analysis/WorkingRepository/Group1/FilterInformationFromERTMSTrackside.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="177">
   <si>
     <t>Template for System Analysis</t>
   </si>
@@ -676,6 +676,9 @@
   </si>
   <si>
     <t>20/11/2013 - v4 - added SysML diagrams</t>
+  </si>
+  <si>
+    <t>DecodedEurobalise</t>
   </si>
 </sst>
 </file>
@@ -1079,15 +1082,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>7</xdr:colOff>
+      <xdr:colOff>361957</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>9537</xdr:rowOff>
+      <xdr:rowOff>28587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>173151</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>3338109</xdr:rowOff>
+      <xdr:colOff>535100</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>13884</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1104,8 +1107,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7" y="7343787"/>
-          <a:ext cx="5507144" cy="3328572"/>
+          <a:off x="361957" y="8448687"/>
+          <a:ext cx="5507143" cy="3328572"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1124,13 +1127,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>162438</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1999208</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>8976</xdr:rowOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>37037</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1147,8 +1150,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="47405925"/>
-          <a:ext cx="8342858" cy="4390476"/>
+          <a:off x="0" y="47568363"/>
+          <a:ext cx="8342858" cy="4065599"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1160,13 +1163,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>601378</xdr:colOff>
       <xdr:row>93</xdr:row>
       <xdr:rowOff>56547</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>694070</xdr:colOff>
+      <xdr:colOff>92692</xdr:colOff>
       <xdr:row>113</xdr:row>
       <xdr:rowOff>95358</xdr:rowOff>
     </xdr:to>
@@ -1185,8 +1188,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="52224972"/>
-          <a:ext cx="10047620" cy="3848811"/>
+          <a:off x="601378" y="52224972"/>
+          <a:ext cx="8844864" cy="3848811"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1486,7 +1489,7 @@
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1680,10 +1683,10 @@
   </sheetPr>
   <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1260" topLeftCell="A94" activePane="bottomLeft"/>
       <selection activeCell="I1" sqref="I1:I1048576"/>
-      <selection pane="bottomLeft" activeCell="H105" sqref="H105"/>
+      <selection pane="bottomLeft" activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2032,7 +2035,7 @@
         <v>68</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F16" s="24" t="s">
         <v>88</v>
@@ -3481,17 +3484,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="G1:G2"/>
@@ -3499,6 +3491,17 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>